<commit_message>
Update file structure for correct images import
Change "images" foder to be in the correct place for images import 14ec51558bfe1af17868e41e14747b942062d3db
</commit_message>
<xml_diff>
--- a/TristanKEREVAL-patch-1/ig/StructureDefinition-Medical-liability-unit.xlsx
+++ b/TristanKEREVAL-patch-1/ig/StructureDefinition-Medical-liability-unit.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://ltsi.univ-rennes.fr/StructureDefinition/MedicalLiabilityUnit</t>
+    <t>http://ltsi.univ-rennes.fr/StructureDefinition/Medical-liability-unit</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-25T09:47:39+00:00</t>
+    <t>2024-03-27T10:49:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>